<commit_message>
Update to fix angular distribution, default parameters, etc.
</commit_message>
<xml_diff>
--- a/11-Parameters/LIONBeamLine-Params-LsrDrvn.xlsx
+++ b/11-Parameters/LIONBeamLine-Params-LsrDrvn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FAC149-90AA-274F-A87D-C373553E6F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131104B8-832F-EA48-BBFF-0927C112E4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15080" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="23340" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LIONBeamLine-Params-LsrDrvn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="86">
   <si>
     <t>Parameter</t>
   </si>
@@ -282,6 +282,18 @@
   </si>
   <si>
     <t>Electron divergence angle</t>
+  </si>
+  <si>
+    <t>SigmaThetaS0</t>
+  </si>
+  <si>
+    <t>SlopeThetaS</t>
+  </si>
+  <si>
+    <t>Intercept of dependence of RMS theta_S on KE</t>
+  </si>
+  <si>
+    <t>Scaled slope of dependence of RMS theta_S on KE</t>
   </si>
 </sst>
 </file>
@@ -332,7 +344,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -435,11 +447,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -458,6 +479,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,9 +499,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -516,7 +539,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -622,7 +645,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -764,7 +787,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -772,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1219,28 +1242,28 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>1</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="3">
         <v>25</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="3" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1249,49 +1272,51 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="14">
+        <v>20</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="15">
         <v>15</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19">
-        <v>4.0340000000000001E-2</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>31</v>
+      <c r="G20" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1302,22 +1327,20 @@
         <v>29</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="3">
-        <v>1.5E-3</v>
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <v>4.0340000000000001E-2</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1328,20 +1351,22 @@
         <v>29</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="F22">
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1352,20 +1377,22 @@
         <v>29</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E23" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F23" s="3">
-        <v>0.04</v>
+        <v>1.5E-3</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1376,20 +1403,20 @@
         <v>29</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="F24" s="3">
-        <v>332</v>
+        <v>0</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1400,22 +1427,20 @@
         <v>29</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="F25" s="3">
-        <v>5.0000000000000001E-3</v>
+        <v>0.04</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1426,20 +1451,20 @@
         <v>29</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="F26" s="3">
-        <v>2.5770000000000001E-2</v>
+        <v>332</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1450,20 +1475,22 @@
         <v>29</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E27" s="3" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="F27" s="3">
-        <v>0.02</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1474,46 +1501,44 @@
         <v>29</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="F28" s="3">
-        <v>318.5</v>
+        <v>2.5770000000000001E-2</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="5">
-        <v>1</v>
-      </c>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="3">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="5">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G29" s="5" t="s">
+      <c r="C29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>43</v>
+      <c r="H29" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1521,47 +1546,49 @@
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="F30" s="3">
-        <v>1.7286520000000001</v>
+        <v>318.5</v>
       </c>
       <c r="G30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
-        <v>1</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="3">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>46</v>
+      <c r="H31" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1572,45 +1599,93 @@
         <v>44</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="F32" s="3">
-        <v>1.5E-3</v>
+        <v>1.7286520000000001</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H32" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1.5E-3</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
-        <v>1</v>
-      </c>
-      <c r="B33" s="5" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>1</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5" t="s">
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F35" s="5">
         <v>0.02</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make datafile format 6 and update tests
</commit_message>
<xml_diff>
--- a/11-Parameters/LIONBeamLine-Params-LsrDrvn.xlsx
+++ b/11-Parameters/LIONBeamLine-Params-LsrDrvn.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D94D9522-70E1-B747-918D-367EFD10D7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC9308E-6536-3646-9CBC-505CC45EB0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="23340" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,7 +191,7 @@
     <t>Max r prime</t>
   </si>
   <si>
-    <t>rpmax-dummy</t>
+    <t>rpmax</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>